<commit_message>
The component refers to the README as source
</commit_message>
<xml_diff>
--- a/Test/VerificationsLog.xlsx
+++ b/Test/VerificationsLog.xlsx
@@ -10,16 +10,16 @@
     <sheet name="Tabelle1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="Test-0275" sheetId="4" r:id="rId4"/>
+    <sheet name="Test-0210-1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
-  <si>
-    <t>0275: Remove any leading or trailing spaces and empt items</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+  <si>
+    <t>0210-1: Array read</t>
   </si>
   <si>
     <t>Verif.
@@ -46,49 +46,46 @@
     <t>01</t>
   </si>
   <si>
-    <t>Empty items are removed</t>
-  </si>
-  <si>
-    <t>Variant()</t>
-  </si>
-  <si>
-    <t>Array</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>Item(0) = 1</t>
+    <t>Read from not-an-array returns Nothing</t>
+  </si>
+  <si>
+    <t>Empty</t>
   </si>
   <si>
     <t xml:space="preserve"> Passed </t>
   </si>
   <si>
-    <t>Item(1) = 2</t>
-  </si>
-  <si>
-    <t>Item(2) = 3</t>
-  </si>
-  <si>
-    <t>Item(3) = 4</t>
-  </si>
-  <si>
-    <t>Item(4) = 5</t>
-  </si>
-  <si>
-    <t>Item(5) = 6</t>
-  </si>
-  <si>
-    <t>Item(6) = 7</t>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Read from a 1-dim array</t>
   </si>
   <si>
     <t>String</t>
   </si>
   <si>
-    <t xml:space="preserve">Item(7) =  , </t>
-  </si>
-  <si>
-    <t>,</t>
+    <t>Item(5)</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>Empty is returned for an index outside the array's dimension specs</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>Read from a 3-dim array</t>
+  </si>
+  <si>
+    <t>Item(1,2)</t>
+  </si>
+  <si>
+    <t>Item(1,2,2)</t>
   </si>
   <si>
     <t xml:space="preserve"> F a i l e d ! </t>
@@ -130,7 +127,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -174,17 +171,6 @@
         <color theme="0" tint="-0.499984740745262"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color theme="0" tint="-0.499984740745262"/>
       </bottom>
@@ -194,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,6 +200,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -223,22 +212,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -582,22 +559,22 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle4"/>
-  <dimension ref="B2:I13"/>
+  <dimension ref="B2:I8"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4:B13"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
@@ -639,190 +616,109 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="7"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="8" t="s">
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="11"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="7"/>
+      <c r="D6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="7">
-        <v>2</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="7">
-        <v>3</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="7">
-        <v>4</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="7">
-        <v>5</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="7">
-        <v>6</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="7">
-        <v>7</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="8" t="s">
+      <c r="D8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="G8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="7"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B4:B13"/>
-    <mergeCell ref="C4:C13"/>
+    <mergeCell ref="C4:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:B4 D3:F3 H3:I3 C4:F4 D5:D6 E6:G6 D7:G13" numberStoredAsText="1"/>
+    <ignoredError sqref="B2:B8 D3:F3 H3:I3 C4:D4 G4:G8 C6:D6 E6:F6 C7:D8 E8:F8 D5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Performance tests for the universal Arry(Let) / write service added
</commit_message>
<xml_diff>
--- a/Test/VerificationsLog.xlsx
+++ b/Test/VerificationsLog.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="214">
   <si>
     <t>Regression Test Summary</t>
   </si>
@@ -33,6 +33,9 @@
 No</t>
   </si>
   <si>
+    <t>Verification Description</t>
+  </si>
+  <si>
     <t>Proc-Type</t>
   </si>
   <si>
@@ -75,7 +78,7 @@
     <t xml:space="preserve"> Passed </t>
   </si>
   <si>
-    <t>502,383</t>
+    <t>512,245</t>
   </si>
   <si>
     <t>02</t>
@@ -126,6 +129,27 @@
     <t>08</t>
   </si>
   <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>An active array item (not IsError and not = default is identified as such</t>
+  </si>
+  <si>
+    <t>ArryItemIsActive</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>An in-active array item (IsError) is identified as such</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>An in-active array item (= default) is identified as such</t>
+  </si>
+  <si>
     <t>0100</t>
   </si>
   <si>
@@ -159,21 +183,12 @@
     <t>Align simple simple right filled with "-"</t>
   </si>
   <si>
-    <t>09</t>
-  </si>
-  <si>
     <t>Align simple centered filled with "-" (not exactly centered)</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>Align simple centered filled with "-" (truncated to 4)</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>Align simple right filled with "-"</t>
   </si>
   <si>
@@ -228,7 +243,7 @@
     <t>ArryNextIndex</t>
   </si>
   <si>
-    <t>0,055</t>
+    <t>0,001</t>
   </si>
   <si>
     <t>The next index for a 1-dim array is the next possible without ReDim</t>
@@ -237,7 +252,7 @@
     <t>Next index for a 1-dim array is not provided because the given has reached the upper bound</t>
   </si>
   <si>
-    <t>0,001</t>
+    <t>0,059</t>
   </si>
   <si>
     <t>Given an index of a 3,4 for a 2-dim 0-4,0-4 array is provided as 4,0</t>
@@ -264,18 +279,27 @@
     <t>Read from a 1-dim array</t>
   </si>
   <si>
+    <t>0,110</t>
+  </si>
+  <si>
     <t>Empty is returned for an index outside the array's dimension specs</t>
   </si>
   <si>
     <t>Read from a 3-dim array</t>
   </si>
   <si>
+    <t>0,205</t>
+  </si>
+  <si>
     <t>Read from a 3-dim array with an index outside the array's dimension specs</t>
   </si>
   <si>
     <t>Return default from a non-existing or not allocated array</t>
   </si>
   <si>
+    <t>0,333</t>
+  </si>
+  <si>
     <t>Return the array's type specific default for an index ouside the bounds of the provided array</t>
   </si>
   <si>
@@ -291,43 +315,55 @@
     <t>0215-1</t>
   </si>
   <si>
-    <t>Write 1-dim Array (results are verified by means of Array-Get)</t>
+    <t>Write 1-dim Array</t>
+  </si>
+  <si>
+    <t>Writing an element to a yet not allocated array without providing an index creates a 1-dim array with one item</t>
+  </si>
+  <si>
+    <t>Arry(Let)</t>
+  </si>
+  <si>
+    <t>Result is verified by means of Array(Get)</t>
   </si>
   <si>
     <t>Writing an element to a yet not allocated array returns a 1-dim array with one Item</t>
   </si>
   <si>
-    <t>Arry(Let)</t>
-  </si>
-  <si>
     <t>Adding an Item to a not yet allocated array with a certain index returns a 1-dim array with one Item at the given index</t>
   </si>
   <si>
+    <t>Adding an Item to an allocated array with a certain index expands the array as required</t>
+  </si>
+  <si>
     <t>0215-2</t>
   </si>
   <si>
     <t>Write to multi-dim array with automated ReDim of any dimensions specs when the requested index is out of bounds</t>
   </si>
   <si>
-    <t>When an index is provided for a multi-dim array an Item is updated when within the bounds</t>
+    <t>When an index is provided for a yet un-dimensioned multi-dim array it is dimensioned with the bounds provided by the indices</t>
   </si>
   <si>
     <t>Write a new item with the last dimensions index beyond its current boundary extents the array</t>
   </si>
   <si>
+    <t>0,795</t>
+  </si>
+  <si>
     <t>Write an item to a yet not dimensioned arry</t>
   </si>
   <si>
-    <t>26,526</t>
+    <t>27,778</t>
   </si>
   <si>
     <t>The multi-dim array created along with writing an item has a from spec based on the "Base Option"</t>
   </si>
   <si>
-    <t>Write an item to an already specifically dimensioned but yet un-allocated array</t>
-  </si>
-  <si>
-    <t>22,385</t>
+    <t>Write an item to an already dimensioned but yet un-allocated array</t>
+  </si>
+  <si>
+    <t>18,938</t>
   </si>
   <si>
     <t>The multi-dim array created along with writing an item has correctly considered the dimensions LBound</t>
@@ -339,9 +375,33 @@
     <t>Writing to a multi-dim array by extending any other but the last dimension re-dims it accordingly</t>
   </si>
   <si>
+    <t>4,701</t>
+  </si>
+  <si>
     <t>Writing with the involment of ArryRedim did not effect any dimensions low bound</t>
   </si>
   <si>
+    <t>0216</t>
+  </si>
+  <si>
+    <t>Performance of writing to an array the usual way versus using the universal Arry service</t>
+  </si>
+  <si>
+    <t>Writing 1000 elements the usual way in a correspondingly dimensioned array</t>
+  </si>
+  <si>
+    <t>0,967</t>
+  </si>
+  <si>
+    <t>Test result is the difference of the exceuton time!</t>
+  </si>
+  <si>
+    <t>Writing 1000 elements by the Arry service</t>
+  </si>
+  <si>
+    <t>209,564</t>
+  </si>
+  <si>
     <t>0220</t>
   </si>
   <si>
@@ -360,6 +420,9 @@
     <t>RngeAsArry</t>
   </si>
   <si>
+    <t>2,087</t>
+  </si>
+  <si>
     <t>The 2-dim array is written to the range not transposed</t>
   </si>
   <si>
@@ -384,6 +447,9 @@
     <t>ArryCompare</t>
   </si>
   <si>
+    <t>0,265</t>
+  </si>
+  <si>
     <t>Compare array with 7th Item not exists in the first one (stop at first difference)</t>
   </si>
   <si>
@@ -402,6 +468,9 @@
     <t>The arrays are equal, empty elements are ignored</t>
   </si>
   <si>
+    <t>0,200</t>
+  </si>
+  <si>
     <t>0240</t>
   </si>
   <si>
@@ -444,15 +513,15 @@
     <t>ArryAsDict</t>
   </si>
   <si>
-    <t>2,072</t>
-  </si>
-  <si>
     <t>The number of items in the array is equal to those in the Dictionary</t>
   </si>
   <si>
     <t>DictAsArray</t>
   </si>
   <si>
+    <t>1,780</t>
+  </si>
+  <si>
     <t>0271</t>
   </si>
   <si>
@@ -474,30 +543,45 @@
     <t>Remove from index 0 two items in an array -2 to 4</t>
   </si>
   <si>
-    <t>0275</t>
+    <t>0275-1</t>
+  </si>
+  <si>
+    <t>Redim array basics</t>
+  </si>
+  <si>
+    <t>Number of items when any = Empty is ignored</t>
+  </si>
+  <si>
+    <t>ArryItems</t>
+  </si>
+  <si>
+    <t>2,124</t>
+  </si>
+  <si>
+    <t>Number of items when any Empty isn't ignored</t>
+  </si>
+  <si>
+    <t>0275-2</t>
   </si>
   <si>
     <t>Redim array</t>
   </si>
   <si>
-    <t>Number of items when any = Empty is ignored</t>
-  </si>
-  <si>
-    <t>ArryReDim</t>
-  </si>
-  <si>
-    <t>Number of items when any Empty isn't ignored</t>
-  </si>
-  <si>
     <t>The resulting array has two more (3) dimensions resulting in 24 items</t>
   </si>
   <si>
-    <t>0,085</t>
+    <t>ArryReDim(S), ArryUnload(F)</t>
+  </si>
+  <si>
+    <t>2,143</t>
   </si>
   <si>
     <t>The resulting array conforms with the expected</t>
   </si>
   <si>
+    <t>4,317</t>
+  </si>
+  <si>
     <t>0280</t>
   </si>
   <si>
@@ -540,18 +624,12 @@
     <t>Coll</t>
   </si>
   <si>
-    <t>0,071</t>
-  </si>
-  <si>
     <t>Read from not existing Collection index</t>
   </si>
   <si>
     <t>Read with existing Collection index</t>
   </si>
   <si>
-    <t>0,048</t>
-  </si>
-  <si>
     <t>Read with not existing Collection index</t>
   </si>
   <si>
@@ -573,16 +651,19 @@
     <t>Write to a very high (10000) index (9998 indices below are filled with Empty)</t>
   </si>
   <si>
-    <t>2,320</t>
+    <t>0,370</t>
   </si>
   <si>
     <t>Read from an existing index</t>
   </si>
   <si>
+    <t>1,003</t>
+  </si>
+  <si>
     <t>Argument is not an integer/index results in the index of the found item</t>
   </si>
   <si>
-    <t>366,443</t>
+    <t>368,466</t>
   </si>
 </sst>
 </file>
@@ -1055,13 +1136,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle4"/>
-  <dimension ref="B2:K104"/>
+  <dimension ref="B2:K111"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4:B11"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,13 +1151,13 @@
     <col min="2" max="2" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="96.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="104.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
@@ -1103,51 +1184,53 @@
       <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="F3" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K4" s="15"/>
     </row>
@@ -1155,25 +1238,25 @@
       <c r="B5" s="13"/>
       <c r="C5" s="20"/>
       <c r="D5" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K5" s="16"/>
     </row>
@@ -1181,25 +1264,25 @@
       <c r="B6" s="13"/>
       <c r="C6" s="20"/>
       <c r="D6" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K6" s="16"/>
     </row>
@@ -1207,25 +1290,25 @@
       <c r="B7" s="13"/>
       <c r="C7" s="20"/>
       <c r="D7" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K7" s="16"/>
     </row>
@@ -1233,25 +1316,25 @@
       <c r="B8" s="13"/>
       <c r="C8" s="20"/>
       <c r="D8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>26</v>
-      </c>
       <c r="I8" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K8" s="16"/>
     </row>
@@ -1259,25 +1342,25 @@
       <c r="B9" s="13"/>
       <c r="C9" s="20"/>
       <c r="D9" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K9" s="16"/>
     </row>
@@ -1285,81 +1368,77 @@
       <c r="B10" s="13"/>
       <c r="C10" s="20"/>
       <c r="D10" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K10" s="16"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="21"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="F11" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K11" s="16"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="19" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>36</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>37</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K12" s="16"/>
     </row>
@@ -1367,77 +1446,81 @@
       <c r="B13" s="13"/>
       <c r="C13" s="20"/>
       <c r="D13" s="7" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>37</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K13" s="16"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="7" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>37</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K14" s="16"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>43</v>
+      </c>
       <c r="D15" s="7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K15" s="16"/>
     </row>
@@ -1445,25 +1528,25 @@
       <c r="B16" s="13"/>
       <c r="C16" s="20"/>
       <c r="D16" s="7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K16" s="16"/>
     </row>
@@ -1471,25 +1554,25 @@
       <c r="B17" s="13"/>
       <c r="C17" s="20"/>
       <c r="D17" s="7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K17" s="16"/>
     </row>
@@ -1497,25 +1580,25 @@
       <c r="B18" s="13"/>
       <c r="C18" s="20"/>
       <c r="D18" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K18" s="16"/>
     </row>
@@ -1523,25 +1606,25 @@
       <c r="B19" s="13"/>
       <c r="C19" s="20"/>
       <c r="D19" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K19" s="16"/>
     </row>
@@ -1549,25 +1632,25 @@
       <c r="B20" s="13"/>
       <c r="C20" s="20"/>
       <c r="D20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="I20" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K20" s="16"/>
     </row>
@@ -1575,25 +1658,25 @@
       <c r="B21" s="13"/>
       <c r="C21" s="20"/>
       <c r="D21" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K21" s="16"/>
     </row>
@@ -1601,81 +1684,77 @@
       <c r="B22" s="13"/>
       <c r="C22" s="20"/>
       <c r="D22" s="7" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K22" s="16"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="14"/>
-      <c r="C23" s="21"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K23" s="16"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="19" t="s">
+      <c r="B24" s="13"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>55</v>
-      </c>
       <c r="F24" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K24" s="16"/>
     </row>
@@ -1683,77 +1762,81 @@
       <c r="B25" s="13"/>
       <c r="C25" s="20"/>
       <c r="D25" s="7" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="16"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="14"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K25" s="16"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>57</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K26" s="16"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="13"/>
-      <c r="C27" s="20"/>
+      <c r="B27" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>59</v>
+      </c>
       <c r="D27" s="7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K27" s="16"/>
     </row>
@@ -1761,25 +1844,25 @@
       <c r="B28" s="13"/>
       <c r="C28" s="20"/>
       <c r="D28" s="7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K28" s="16"/>
     </row>
@@ -1787,25 +1870,25 @@
       <c r="B29" s="13"/>
       <c r="C29" s="20"/>
       <c r="D29" s="7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K29" s="16"/>
     </row>
@@ -1813,25 +1896,25 @@
       <c r="B30" s="13"/>
       <c r="C30" s="20"/>
       <c r="D30" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K30" s="16"/>
     </row>
@@ -1839,25 +1922,25 @@
       <c r="B31" s="13"/>
       <c r="C31" s="20"/>
       <c r="D31" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K31" s="16"/>
     </row>
@@ -1865,25 +1948,25 @@
       <c r="B32" s="13"/>
       <c r="C32" s="20"/>
       <c r="D32" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="I32" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K32" s="16"/>
     </row>
@@ -1891,25 +1974,25 @@
       <c r="B33" s="13"/>
       <c r="C33" s="20"/>
       <c r="D33" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K33" s="16"/>
     </row>
@@ -1917,81 +2000,77 @@
       <c r="B34" s="13"/>
       <c r="C34" s="20"/>
       <c r="D34" s="7" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J34" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K34" s="16"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="14"/>
-      <c r="C35" s="21"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="20"/>
       <c r="D35" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K35" s="16"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>65</v>
-      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="20"/>
       <c r="D36" s="7" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" s="10" t="s">
-        <v>68</v>
+        <v>17</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="K36" s="16"/>
     </row>
@@ -1999,107 +2078,107 @@
       <c r="B37" s="13"/>
       <c r="C37" s="20"/>
       <c r="D37" s="7" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="E37" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K37" s="16"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="14"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38" s="16"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F37" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J37" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K37" s="16"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="13"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" s="8" t="s">
+      <c r="C39" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F38" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J38" s="10" t="s">
+      <c r="D39" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K38" s="16"/>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="14"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E39" s="8" t="s">
+      <c r="F39" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F39" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="I39" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K39" s="16"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" s="19" t="s">
+      <c r="B40" s="13"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="F40" s="8" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K40" s="16"/>
     </row>
@@ -2107,77 +2186,81 @@
       <c r="B41" s="13"/>
       <c r="C41" s="20"/>
       <c r="D41" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E41" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="K41" s="16"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="14"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K42" s="16"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="F41" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="I41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J41" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K41" s="16"/>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="13"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E42" s="8" t="s">
+      <c r="C43" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="F42" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="I42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J42" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="K42" s="16"/>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="13"/>
-      <c r="C43" s="20"/>
       <c r="D43" s="7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>80</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J43" s="10" t="s">
-        <v>71</v>
+        <v>17</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="K43" s="16"/>
     </row>
@@ -2185,25 +2268,25 @@
       <c r="B44" s="13"/>
       <c r="C44" s="20"/>
       <c r="D44" s="7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E44" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F44" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F44" s="8" t="s">
-        <v>76</v>
-      </c>
       <c r="G44" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J44" s="10" t="s">
-        <v>71</v>
+        <v>17</v>
+      </c>
+      <c r="J44" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="K44" s="16"/>
     </row>
@@ -2211,25 +2294,25 @@
       <c r="B45" s="13"/>
       <c r="C45" s="20"/>
       <c r="D45" s="7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E45" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F45" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="I45" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="K45" s="16"/>
     </row>
@@ -2237,25 +2320,25 @@
       <c r="B46" s="13"/>
       <c r="C46" s="20"/>
       <c r="D46" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K46" s="16"/>
     </row>
@@ -2263,25 +2346,25 @@
       <c r="B47" s="13"/>
       <c r="C47" s="20"/>
       <c r="D47" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="K47" s="16"/>
     </row>
@@ -2289,25 +2372,25 @@
       <c r="B48" s="13"/>
       <c r="C48" s="20"/>
       <c r="D48" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K48" s="16"/>
     </row>
@@ -2315,189 +2398,187 @@
       <c r="B49" s="13"/>
       <c r="C49" s="20"/>
       <c r="D49" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J49" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="K49" s="16"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="14"/>
-      <c r="C50" s="21"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="20"/>
       <c r="D50" s="7" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J50" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="K50" s="16"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>89</v>
-      </c>
+      <c r="B51" s="13"/>
+      <c r="C51" s="20"/>
       <c r="D51" s="7" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K51" s="16"/>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="14"/>
-      <c r="C52" s="21"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="20"/>
       <c r="D52" s="7" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J52" s="10" t="s">
-        <v>71</v>
+        <v>17</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="K52" s="16"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C53" s="19" t="s">
-        <v>94</v>
-      </c>
+      <c r="B53" s="14"/>
+      <c r="C53" s="21"/>
       <c r="D53" s="7" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>95</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K53" s="16"/>
+        <v>21</v>
+      </c>
+      <c r="K53" s="17"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="13"/>
-      <c r="C54" s="20"/>
+      <c r="B54" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>97</v>
+      </c>
       <c r="D54" s="7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="K54" s="16"/>
+        <v>73</v>
+      </c>
+      <c r="K54" s="15" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="13"/>
       <c r="C55" s="20"/>
       <c r="D55" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="K55" s="16"/>
     </row>
@@ -2505,77 +2586,81 @@
       <c r="B56" s="13"/>
       <c r="C56" s="20"/>
       <c r="D56" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E56" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H56" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F56" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H56" s="9" t="s">
-        <v>91</v>
-      </c>
       <c r="I56" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J56" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="J56" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="K56" s="16"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="13"/>
-      <c r="C57" s="20"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="21"/>
       <c r="D57" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="K57" s="16"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="13"/>
-      <c r="C58" s="20"/>
+      <c r="B58" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>105</v>
+      </c>
       <c r="D58" s="7" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K58" s="16"/>
     </row>
@@ -2583,25 +2668,25 @@
       <c r="B59" s="13"/>
       <c r="C59" s="20"/>
       <c r="D59" s="7" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H59" s="9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="K59" s="16"/>
     </row>
@@ -2609,293 +2694,299 @@
       <c r="B60" s="13"/>
       <c r="C60" s="20"/>
       <c r="D60" s="7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H60" s="9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="K60" s="16"/>
+        <v>110</v>
+      </c>
+      <c r="K60" s="17"/>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B61" s="14"/>
-      <c r="C61" s="21"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="20"/>
       <c r="D61" s="7" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J61" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K61" s="16"/>
+        <v>21</v>
+      </c>
+      <c r="K61" s="8"/>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C62" s="19" t="s">
-        <v>107</v>
-      </c>
+      <c r="B62" s="13"/>
+      <c r="C62" s="20"/>
       <c r="D62" s="7" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H62" s="9" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="K62" s="16"/>
+        <v>113</v>
+      </c>
+      <c r="K62" s="8" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" s="13"/>
       <c r="C63" s="20"/>
       <c r="D63" s="7" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H63" s="9" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="I63" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J63" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="K63" s="16"/>
+        <v>17</v>
+      </c>
+      <c r="J63" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K63" s="15"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" s="13"/>
       <c r="C64" s="20"/>
       <c r="D64" s="7" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H64" s="9" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="I64" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="K64" s="16"/>
+        <v>73</v>
+      </c>
+      <c r="K64" s="17"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B65" s="14"/>
-      <c r="C65" s="21"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="20"/>
       <c r="D65" s="7" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="K65" s="16"/>
+        <v>117</v>
+      </c>
+      <c r="K65" s="8" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B66" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>117</v>
-      </c>
+      <c r="B66" s="14"/>
+      <c r="C66" s="21"/>
       <c r="D66" s="7" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>118</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="G66" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="I66" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J66" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K66" s="8"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="I67" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J67" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="K67" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="14"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="I68" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J68" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="K68" s="17"/>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F69" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H66" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="I66" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J66" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="K66" s="16"/>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B67" s="13"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G67" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H67" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="I67" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J67" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K67" s="16"/>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B68" s="13"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G68" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H68" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="I68" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J68" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="K68" s="16"/>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B69" s="13"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="F69" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="G69" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J69" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K69" s="16"/>
+        <v>17</v>
+      </c>
+      <c r="J69" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K69" s="15"/>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" s="13"/>
       <c r="C70" s="20"/>
       <c r="D70" s="7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="I70" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J70" s="10" t="s">
-        <v>71</v>
+        <v>132</v>
       </c>
       <c r="K70" s="16"/>
     </row>
@@ -2903,25 +2994,25 @@
       <c r="B71" s="13"/>
       <c r="C71" s="20"/>
       <c r="D71" s="7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H71" s="9" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J71" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K71" s="16"/>
     </row>
@@ -2929,55 +3020,55 @@
       <c r="B72" s="14"/>
       <c r="C72" s="21"/>
       <c r="D72" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H72" s="9" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J72" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K72" s="16"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B73" s="12" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H73" s="9" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J73" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="J73" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="K73" s="16"/>
     </row>
@@ -2985,135 +3076,129 @@
       <c r="B74" s="13"/>
       <c r="C74" s="20"/>
       <c r="D74" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="I74" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J74" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K74" s="16"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B75" s="13"/>
-      <c r="C75" s="21"/>
+      <c r="C75" s="20"/>
       <c r="D75" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H75" s="9" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="I75" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J75" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="J75" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="K75" s="16"/>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" s="13"/>
-      <c r="C76" s="19" t="s">
-        <v>132</v>
-      </c>
+      <c r="C76" s="20"/>
       <c r="D76" s="7" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H76" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="I76" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K76" s="16"/>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B77" s="13"/>
+      <c r="C77" s="20"/>
+      <c r="D77" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F77" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="I76" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J76" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K76" s="16"/>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B77" s="14"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F77" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="G77" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H77" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="I77" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J77" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K77" s="16"/>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B78" s="13"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F78" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="I77" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J77" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K77" s="16"/>
-    </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B78" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="C78" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="G78" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I78" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J78" s="10" t="s">
-        <v>140</v>
+        <v>73</v>
       </c>
       <c r="K78" s="16"/>
     </row>
@@ -3121,53 +3206,55 @@
       <c r="B79" s="14"/>
       <c r="C79" s="21"/>
       <c r="D79" s="7" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H79" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I79" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J79" s="10" t="s">
-        <v>71</v>
+        <v>148</v>
       </c>
       <c r="K79" s="16"/>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="C80" s="19"/>
+        <v>149</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>150</v>
+      </c>
       <c r="D80" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H80" s="9" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J80" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K80" s="16"/>
     </row>
@@ -3175,77 +3262,79 @@
       <c r="B81" s="13"/>
       <c r="C81" s="20"/>
       <c r="D81" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H81" s="9" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="I81" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J81" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K81" s="16"/>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B82" s="13"/>
-      <c r="C82" s="20"/>
+      <c r="C82" s="21"/>
       <c r="D82" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H82" s="9" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="I82" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J82" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K82" s="16"/>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B83" s="13"/>
-      <c r="C83" s="20"/>
+      <c r="C83" s="19" t="s">
+        <v>155</v>
+      </c>
       <c r="D83" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H83" s="9" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="I83" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J83" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K83" s="16"/>
     </row>
@@ -3253,107 +3342,109 @@
       <c r="B84" s="14"/>
       <c r="C84" s="21"/>
       <c r="D84" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H84" s="9" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="I84" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J84" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K84" s="16"/>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B85" s="12" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H85" s="9" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="I85" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J85" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K85" s="16"/>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B86" s="13"/>
-      <c r="C86" s="20"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="21"/>
       <c r="D86" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="G86" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H86" s="9" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J86" s="10" t="s">
-        <v>71</v>
+        <v>165</v>
       </c>
       <c r="K86" s="16"/>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B87" s="13"/>
-      <c r="C87" s="20"/>
+      <c r="B87" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C87" s="19"/>
       <c r="D87" s="7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H87" s="9" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J87" s="10" t="s">
-        <v>156</v>
+        <v>17</v>
+      </c>
+      <c r="J87" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="K87" s="16"/>
     </row>
@@ -3361,193 +3452,189 @@
       <c r="B88" s="13"/>
       <c r="C88" s="20"/>
       <c r="D88" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="G88" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H88" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="I88" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J88" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K88" s="16"/>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B89" s="13"/>
+      <c r="C89" s="20"/>
+      <c r="D89" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E89" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F89" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G89" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H89" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="I89" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J89" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K89" s="16"/>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B90" s="13"/>
+      <c r="C90" s="20"/>
+      <c r="D90" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E90" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F90" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G90" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H90" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="I90" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J90" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K90" s="16"/>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B91" s="14"/>
+      <c r="C91" s="21"/>
+      <c r="D91" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E91" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="F91" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G91" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H91" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="I91" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J91" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K91" s="16"/>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B92" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C92" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E92" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F92" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G92" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H92" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="I92" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J92" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="K92" s="16"/>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B93" s="14"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F93" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G93" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H93" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="I93" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J93" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K93" s="16"/>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B94" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C94" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F94" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H88" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="I88" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J88" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="K88" s="16"/>
-    </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B89" s="14"/>
-      <c r="C89" s="21"/>
-      <c r="D89" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E89" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="F89" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G89" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H89" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="I89" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J89" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K89" s="16"/>
-    </row>
-    <row r="90" spans="2:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="B90" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C90" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E90" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="F90" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G90" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H90" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="I90" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J90" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K90" s="16"/>
-    </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B91" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C91" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E91" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F91" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G91" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H91" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="I91" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J91" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K91" s="16"/>
-    </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B92" s="14"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E92" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="F92" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G92" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H92" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="I92" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J92" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K92" s="16"/>
-    </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B93" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C93" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E93" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F93" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="G93" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H93" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="I93" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J93" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="K93" s="16"/>
-    </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B94" s="13"/>
-      <c r="C94" s="20"/>
-      <c r="D94" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E94" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="F94" s="8" t="s">
-        <v>170</v>
-      </c>
       <c r="G94" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H94" s="9" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="I94" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J94" s="10" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
       <c r="K94" s="16"/>
     </row>
@@ -3555,155 +3642,167 @@
       <c r="B95" s="13"/>
       <c r="C95" s="20"/>
       <c r="D95" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>170</v>
+        <v>14</v>
       </c>
       <c r="G95" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H95" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="I95" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J95" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="K95" s="16"/>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B96" s="14"/>
+      <c r="C96" s="21"/>
+      <c r="D96" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E96" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F96" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H95" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="I95" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J95" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="K95" s="16"/>
-    </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B96" s="13"/>
-      <c r="C96" s="20"/>
-      <c r="D96" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="F96" s="8" t="s">
-        <v>170</v>
-      </c>
       <c r="G96" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H96" s="9" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J96" s="10" t="s">
-        <v>71</v>
+        <v>17</v>
+      </c>
+      <c r="J96" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="K96" s="16"/>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B97" s="13"/>
-      <c r="C97" s="20"/>
+    <row r="97" spans="2:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="B97" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C97" s="22" t="s">
+        <v>187</v>
+      </c>
       <c r="D97" s="7" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H97" s="9" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J97" s="10" t="s">
-        <v>71</v>
+        <v>17</v>
+      </c>
+      <c r="J97" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="K97" s="16"/>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B98" s="13"/>
-      <c r="C98" s="20"/>
+      <c r="B98" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C98" s="19" t="s">
+        <v>191</v>
+      </c>
       <c r="D98" s="7" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>170</v>
+        <v>26</v>
       </c>
       <c r="G98" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H98" s="9" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J98" s="10" t="s">
-        <v>71</v>
+        <v>17</v>
+      </c>
+      <c r="J98" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="K98" s="16"/>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B99" s="13"/>
-      <c r="C99" s="20"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="21"/>
       <c r="D99" s="7" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>170</v>
+        <v>26</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H99" s="9" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J99" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K99" s="16"/>
     </row>
     <row r="100" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B100" s="13"/>
-      <c r="C100" s="20"/>
+      <c r="B100" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C100" s="19" t="s">
+        <v>196</v>
+      </c>
       <c r="D100" s="7" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H100" s="9" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="I100" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J100" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="J100" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="K100" s="16"/>
     </row>
@@ -3711,25 +3810,25 @@
       <c r="B101" s="13"/>
       <c r="C101" s="20"/>
       <c r="D101" s="7" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H101" s="9" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="I101" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J101" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="J101" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="K101" s="16"/>
     </row>
@@ -3737,25 +3836,25 @@
       <c r="B102" s="13"/>
       <c r="C102" s="20"/>
       <c r="D102" s="7" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="G102" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H102" s="9" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="I102" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J102" s="10" t="s">
-        <v>183</v>
+        <v>73</v>
       </c>
       <c r="K102" s="16"/>
     </row>
@@ -3763,93 +3862,283 @@
       <c r="B103" s="13"/>
       <c r="C103" s="20"/>
       <c r="D103" s="7" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="G103" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H103" s="9" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="I103" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J103" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K103" s="16"/>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B104" s="14"/>
-      <c r="C104" s="21"/>
+      <c r="B104" s="13"/>
+      <c r="C104" s="20"/>
       <c r="D104" s="7" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="G104" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H104" s="9" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="I104" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J104" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="K104" s="17"/>
+        <v>73</v>
+      </c>
+      <c r="K104" s="16"/>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B105" s="13"/>
+      <c r="C105" s="20"/>
+      <c r="D105" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E105" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="F105" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G105" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H105" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="I105" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J105" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K105" s="16"/>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B106" s="13"/>
+      <c r="C106" s="20"/>
+      <c r="D106" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F106" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G106" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H106" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="I106" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J106" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K106" s="16"/>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B107" s="13"/>
+      <c r="C107" s="20"/>
+      <c r="D107" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E107" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F107" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G107" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H107" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="I107" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J107" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K107" s="16"/>
+    </row>
+    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B108" s="13"/>
+      <c r="C108" s="20"/>
+      <c r="D108" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E108" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F108" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G108" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H108" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="I108" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J108" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K108" s="16"/>
+    </row>
+    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B109" s="13"/>
+      <c r="C109" s="20"/>
+      <c r="D109" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E109" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F109" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G109" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H109" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="I109" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J109" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="K109" s="16"/>
+    </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B110" s="13"/>
+      <c r="C110" s="20"/>
+      <c r="D110" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E110" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="F110" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G110" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H110" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="I110" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J110" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="K110" s="16"/>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B111" s="14"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E111" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="F111" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G111" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H111" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="I111" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J111" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="K111" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="C80:C84"/>
-    <mergeCell ref="C85:C89"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="C93:C104"/>
-    <mergeCell ref="K4:K104"/>
-    <mergeCell ref="C53:C61"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C66:C72"/>
-    <mergeCell ref="C73:C75"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="C78:C79"/>
+  <mergeCells count="41">
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="C100:C111"/>
+    <mergeCell ref="K4:K53"/>
+    <mergeCell ref="K54:K60"/>
+    <mergeCell ref="K63:K64"/>
+    <mergeCell ref="K67:K68"/>
+    <mergeCell ref="K69:K111"/>
+    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C87:C91"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="C94:C96"/>
+    <mergeCell ref="C43:C53"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C58:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C72"/>
+    <mergeCell ref="C73:C79"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="B94:B96"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="B100:B111"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="B58:B66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="B69:B72"/>
+    <mergeCell ref="B73:B79"/>
     <mergeCell ref="B80:B84"/>
-    <mergeCell ref="B85:B89"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="B93:B104"/>
-    <mergeCell ref="C4:C11"/>
-    <mergeCell ref="C12:C23"/>
-    <mergeCell ref="C24:C35"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B61"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="B66:B72"/>
-    <mergeCell ref="B73:B77"/>
-    <mergeCell ref="B78:B79"/>
     <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B4:B11"/>
-    <mergeCell ref="B12:B23"/>
-    <mergeCell ref="B24:B35"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B50"/>
+    <mergeCell ref="B4:B14"/>
+    <mergeCell ref="B15:B26"/>
+    <mergeCell ref="B27:B38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B43:B53"/>
+    <mergeCell ref="C4:C14"/>
+    <mergeCell ref="C15:C26"/>
+    <mergeCell ref="C27:C38"/>
+    <mergeCell ref="C39:C42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:B4 C3:D3 F3:H3 J3:K3 C4:J4 D80:J84 C85:J85 B12 B24 B36 B40 B51 B53 B62 B66 B73 B78 B80 B85 B90:B91 B93 C12:J12 D5:J11 C24:J24 D13:J23 C36:J36 D25:J35 C40:J40 D37:J39 C51:J51 D41:J50 C53:J53 D52:J52 C62:J62 D54:J61 C66:J66 D63:J65 C73:J73 D67:J72 C76:J76 D74:J75 C78:J78 D77:J77 D79:J79 C90:J91 D86:J89 C93:J93 D92:J92 D94:J104" numberStoredAsText="1"/>
+    <ignoredError sqref="B2:B4 C3:H3 J3:K3 C4:J4 K54 C58:J58 K62 D63:J65 K65 C67:J67 K67 C69:J69 D87:J91 C92:J92 B15 B27 B39 B43 B54 B58 B67 B69 B73 B80 B85 B87 B92 B94 B97:B98 B100 C15:J15 D5:J14 C27:J27 D16:J26 C39:J39 D28:J38 C43:J43 D40:J42 C54:J54 D44:J53 D55:J57 D59:J62 D66:J66 D68:J68 C73:J73 D70:J72 C80:J80 D74:J79 C83:J83 D81:J82 C85:J85 D84:J84 D86:J86 C94:J94 D93:J93 C97:J98 D95:J96 C100:J100 D99:J99 D101:J111" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>